<commit_message>
feat: create/drop db + ER update
</commit_message>
<xml_diff>
--- a/Filegroups_support.xlsx
+++ b/Filegroups_support.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\wwi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6520E1F9-A91C-4950-90E4-83BBA046F23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F143AF-D945-4BED-AA79-2F17505A9DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{060E0144-75C7-4C12-B4D9-C7F9369402C2}"/>
   </bookViews>
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -379,28 +379,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C2F128-56C4-4A17-AFB6-7B93C606ECA2}">
-  <dimension ref="A1:S72"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59:M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,158 +730,143 @@
     <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10">
         <v>19</v>
       </c>
       <c r="J2" s="3">
         <f>SUM(J3:J6)</f>
         <v>494</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
       <c r="R2" s="3">
         <f>SUM(R3:R6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="13" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3">
         <v>19</v>
       </c>
       <c r="J3" s="5">
         <f>PRODUCT(I3,H3)</f>
         <v>76</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="24"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
       <c r="R3" s="5">
         <f>PRODUCT(Q3,P3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="5">
         <v>8</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="13" t="s">
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4">
         <f>(12+2)</f>
         <v>14</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4">
         <v>19</v>
       </c>
       <c r="J4" s="5">
         <f>PRODUCT(I4,H4)</f>
         <v>266</v>
       </c>
-      <c r="K4" s="13"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
       <c r="R4" s="5">
         <f>PRODUCT(Q4,P4)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="14"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -899,35 +874,29 @@
         <v>4</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="13" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5">
         <v>6</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5">
         <v>19</v>
       </c>
       <c r="J5" s="5">
         <f>PRODUCT(I5,H5)</f>
         <v>114</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
       <c r="R5" s="5">
         <f>PRODUCT(Q5,P5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -935,35 +904,29 @@
         <v>2</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="16" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6">
         <v>19</v>
       </c>
       <c r="J6" s="5">
         <f>PRODUCT(I6,H6)</f>
         <v>38</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
       <c r="R6" s="5">
         <f>PRODUCT(Q6,P6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -971,34 +934,24 @@
         <v>1</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="16">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10">
         <v>10</v>
       </c>
       <c r="J8" s="3">
@@ -1006,33 +959,29 @@
         <v>140</v>
       </c>
       <c r="M8" s="2"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="16"/>
       <c r="R8" s="3">
         <f>SUM(R9:R11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="16" t="s">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9">
         <v>4</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9">
         <f>I8</f>
         <v>10</v>
       </c>
@@ -1041,33 +990,29 @@
         <v>40</v>
       </c>
       <c r="M9" s="4"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="16"/>
       <c r="R9" s="5">
         <f>PRODUCT(Q9,P9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="5">
         <v>3</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="16" t="s">
+      <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10">
         <f>I9</f>
         <v>10</v>
       </c>
@@ -1076,31 +1021,26 @@
         <v>10</v>
       </c>
       <c r="M10" s="4"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
       <c r="R10" s="5">
         <f>PRODUCT(Q10,P10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="5">
         <v>8</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="16" t="s">
+      <c r="F11" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16">
+      <c r="H11">
         <v>9</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11">
         <f>I10</f>
         <v>10</v>
       </c>
@@ -1109,37 +1049,25 @@
         <v>90</v>
       </c>
       <c r="M11" s="4"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
       <c r="R11" s="5">
         <f>PRODUCT(Q11,P11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
       <c r="J12" s="5"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="7">
@@ -1148,10 +1076,10 @@
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10">
         <v>9</v>
       </c>
       <c r="J13" s="3">
@@ -1159,27 +1087,23 @@
         <v>126</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
       <c r="R13" s="3">
         <f xml:space="preserve"> SUM(R14:R15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E14" s="4"/>
-      <c r="F14" s="16" t="s">
+      <c r="F14" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14">
         <v>4</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14">
         <v>9</v>
       </c>
       <c r="J14" s="5">
@@ -1187,27 +1111,23 @@
         <v>36</v>
       </c>
       <c r="M14" s="4"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="13"/>
       <c r="R14" s="5">
         <f>PRODUCT(Q13,P14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" s="4"/>
-      <c r="F15" s="16" t="s">
+      <c r="F15" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15">
         <v>10</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15">
         <v>9</v>
       </c>
       <c r="J15" s="5">
@@ -1215,24 +1135,18 @@
         <v>90</v>
       </c>
       <c r="M15" s="4"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
       <c r="R15" s="5">
         <f>PRODUCT(Q15,P15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="I16" s="13"/>
+      <c r="E16" s="4"/>
       <c r="J16" s="5"/>
       <c r="M16" s="6"/>
-      <c r="Q16" s="13"/>
       <c r="R16" s="5"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1242,7 +1156,10 @@
       <c r="E17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="13">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10">
         <v>23272</v>
       </c>
       <c r="J17" s="3">
@@ -1250,7 +1167,6 @@
         <v>325808</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="Q17" s="13"/>
       <c r="R17" s="3">
         <f>SUM(R18:R19)</f>
         <v>0</v>
@@ -1273,7 +1189,7 @@
       <c r="H18">
         <v>4</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18">
         <v>23272</v>
       </c>
       <c r="J18" s="5">
@@ -1281,14 +1197,13 @@
         <v>93088</v>
       </c>
       <c r="M18" s="4"/>
-      <c r="Q18" s="13"/>
       <c r="R18" s="5">
         <f>(P18*Q18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="5">
@@ -1304,7 +1219,7 @@
       <c r="H19">
         <v>10</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19">
         <v>23272</v>
       </c>
       <c r="J19" s="5">
@@ -1312,7 +1227,6 @@
         <v>232720</v>
       </c>
       <c r="M19" s="4"/>
-      <c r="Q19" s="13"/>
       <c r="R19" s="5">
         <f>(P19*Q19)</f>
         <v>0</v>
@@ -1325,8 +1239,8 @@
       <c r="B20" s="5">
         <v>9</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="J20" s="7"/>
+      <c r="E20" s="4"/>
+      <c r="J20" s="5"/>
       <c r="M20" s="6"/>
       <c r="R20" s="7"/>
     </row>
@@ -1337,18 +1251,21 @@
       <c r="B21" s="5">
         <v>13</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I21">
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10">
         <v>1</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="3">
         <f>SUM(J22:J23)</f>
         <v>16</v>
       </c>
-      <c r="M21" s="22"/>
-      <c r="R21" s="26">
+      <c r="M21" s="13"/>
+      <c r="R21" s="15">
         <f>SUM(R22:R23)</f>
         <v>0</v>
       </c>
@@ -1411,37 +1328,40 @@
       <c r="A24" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="4"/>
       <c r="J24" s="7"/>
       <c r="M24" s="6"/>
       <c r="R24" s="7"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="E25" s="22" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="E25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I25">
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10">
         <v>1</v>
       </c>
-      <c r="J25" s="26">
+      <c r="J25" s="15">
         <f>SUM(J26:J28)</f>
         <v>20</v>
       </c>
-      <c r="M25" s="22"/>
-      <c r="R25" s="26">
+      <c r="M25" s="13"/>
+      <c r="R25" s="15">
         <f>SUM(R26:R28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
       <c r="E26" s="4"/>
       <c r="F26" t="s">
         <v>24</v>
@@ -1466,9 +1386,9 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
       <c r="E27" s="4"/>
       <c r="F27" t="s">
         <v>19</v>
@@ -1520,18 +1440,21 @@
       <c r="R29" s="7"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I30">
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10">
         <v>53</v>
       </c>
-      <c r="J30" s="26">
+      <c r="J30" s="15">
         <f>SUM(J31:J34)</f>
         <v>901</v>
       </c>
-      <c r="M30" s="22"/>
-      <c r="R30" s="26">
+      <c r="M30" s="13"/>
+      <c r="R30" s="15">
         <f>SUM(R31:R34)</f>
         <v>0</v>
       </c>
@@ -1635,19 +1558,22 @@
       <c r="R35" s="7"/>
     </row>
     <row r="36" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I36">
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10">
         <f>I17</f>
         <v>23272</v>
       </c>
-      <c r="J36" s="26">
+      <c r="J36" s="15">
         <f>SUM(J37:J41)</f>
         <v>349080</v>
       </c>
-      <c r="M36" s="22"/>
-      <c r="R36" s="26">
+      <c r="M36" s="13"/>
+      <c r="R36" s="15">
         <f>SUM(R37:R41)</f>
         <v>0</v>
       </c>
@@ -1767,13 +1693,16 @@
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I43">
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10">
         <v>317</v>
       </c>
-      <c r="J43" s="18">
+      <c r="J43" s="11">
         <v>1268</v>
       </c>
     </row>
@@ -1805,17 +1734,20 @@
       <c r="J46" s="5"/>
     </row>
     <row r="47" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E47" s="27"/>
+      <c r="E47" s="6"/>
       <c r="J47" s="7"/>
     </row>
     <row r="48" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E48" s="22" t="s">
+      <c r="E48" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I48">
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10">
         <v>5</v>
       </c>
-      <c r="J48" s="26">
+      <c r="J48" s="15">
         <f>SUM(J49:J50)</f>
         <v>70</v>
       </c>
@@ -1867,7 +1799,11 @@
       <c r="E52" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J52" s="18"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="11"/>
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E53" s="4"/>
@@ -1888,56 +1824,135 @@
       <c r="J55" s="5"/>
     </row>
     <row r="56" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E56" s="4"/>
-      <c r="J56" s="5"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J57" s="5"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J58" s="5"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
     </row>
     <row r="59" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J59" s="5"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
     </row>
     <row r="60" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J60" s="5"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
     </row>
     <row r="61" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J61" s="5"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17"/>
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J62" s="5"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
     </row>
     <row r="63" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J63" s="5"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
     </row>
     <row r="64" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J72" s="5"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="17"/>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="17"/>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+      <c r="J70" s="17"/>
+    </row>
+    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+      <c r="J71" s="17"/>
+    </row>
+    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J72" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>